<commit_message>
code is update and fix
</commit_message>
<xml_diff>
--- a/Results_BEFORE_filled.xlsx
+++ b/Results_BEFORE_filled.xlsx
@@ -711,10 +711,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9797</v>
+        <v>0.9789</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9792</v>
+        <v>0.9782999999999999</v>
       </c>
       <c r="D6" t="n">
         <v>0.9875</v>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>C=10</t>
+          <t>C=1</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>C=1</t>
+          <t>C=10</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>C=10</t>
+          <t>C=1</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3527,10 +3527,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.9789</v>
+        <v>0.9781</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9586</v>
+        <v>0.9577</v>
       </c>
       <c r="D54" t="n">
         <v>0.9867</v>
@@ -3775,10 +3775,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.9781</v>
+        <v>0.9772999999999999</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9735</v>
+        <v>0.9726</v>
       </c>
       <c r="D58" t="n">
         <v>0.9844000000000001</v>
@@ -4541,10 +4541,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.9812</v>
+        <v>0.9804</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9607</v>
+        <v>0.9598</v>
       </c>
       <c r="D71" t="n">
         <v>0.9836</v>
@@ -4748,61 +4748,6 @@
           <t>Fold 1</t>
         </is>
       </c>
-      <c r="B75" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0.9825</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="E75" t="n">
-        <v>0.7294</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G75" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" t="n">
-        <v>0.9797</v>
-      </c>
-      <c r="K75" t="n">
-        <v>0.7302999999999999</v>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4810,61 +4755,6 @@
           <t>Fold 2</t>
         </is>
       </c>
-      <c r="B76" t="n">
-        <v>0.9797</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.9792</v>
-      </c>
-      <c r="D76" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0.7211</v>
-      </c>
-      <c r="F76" t="n">
-        <v>1</v>
-      </c>
-      <c r="G76" t="n">
-        <v>1</v>
-      </c>
-      <c r="H76" t="n">
-        <v>1</v>
-      </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="n">
-        <v>0.9797</v>
-      </c>
-      <c r="K76" t="n">
-        <v>0.9734</v>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4872,61 +4762,6 @@
           <t>Fold 3</t>
         </is>
       </c>
-      <c r="B77" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0.9786</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0.9859</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0.731</v>
-      </c>
-      <c r="F77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0.9977</v>
-      </c>
-      <c r="I77" t="n">
-        <v>0.9977</v>
-      </c>
-      <c r="J77" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0.7318</v>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4934,61 +4769,6 @@
           <t>Fold 4</t>
         </is>
       </c>
-      <c r="B78" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0.9842</v>
-      </c>
-      <c r="D78" t="n">
-        <v>0.9883</v>
-      </c>
-      <c r="E78" t="n">
-        <v>0.9784</v>
-      </c>
-      <c r="F78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G78" t="n">
-        <v>1</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I78" t="n">
-        <v>0.9985000000000001</v>
-      </c>
-      <c r="J78" t="n">
-        <v>0.9851</v>
-      </c>
-      <c r="K78" t="n">
-        <v>0.7327</v>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
-        <is>
-          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4996,61 +4776,6 @@
           <t>Fold 5</t>
         </is>
       </c>
-      <c r="B79" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0.7333</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0.9875</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0.7383999999999999</v>
-      </c>
-      <c r="F79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H79" t="n">
-        <v>1</v>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="K79" t="n">
-        <v>0.7314000000000001</v>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>n_neighbors=5; weights=distance</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5058,61 +4783,6 @@
           <t>Fold 6</t>
         </is>
       </c>
-      <c r="B80" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0.9694</v>
-      </c>
-      <c r="D80" t="n">
-        <v>0.9804</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0.9707</v>
-      </c>
-      <c r="F80" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" t="n">
-        <v>1</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0.9985000000000001</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0.9687</v>
-      </c>
-      <c r="K80" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5120,61 +4790,6 @@
           <t>Fold 7</t>
         </is>
       </c>
-      <c r="B81" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="C81" t="n">
-        <v>0.7229</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="E81" t="n">
-        <v>0.7272999999999999</v>
-      </c>
-      <c r="F81" t="n">
-        <v>1</v>
-      </c>
-      <c r="G81" t="n">
-        <v>1</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0.7463</v>
-      </c>
-      <c r="J81" t="n">
-        <v>0.9772999999999999</v>
-      </c>
-      <c r="K81" t="n">
-        <v>0.7238</v>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5182,61 +4797,6 @@
           <t>Fold 8</t>
         </is>
       </c>
-      <c r="B82" t="n">
-        <v>0.9789</v>
-      </c>
-      <c r="C82" t="n">
-        <v>0.972</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0.9789</v>
-      </c>
-      <c r="E82" t="n">
-        <v>0.7013</v>
-      </c>
-      <c r="F82" t="n">
-        <v>1</v>
-      </c>
-      <c r="G82" t="n">
-        <v>1</v>
-      </c>
-      <c r="H82" t="n">
-        <v>1</v>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="n">
-        <v>0.9703000000000001</v>
-      </c>
-      <c r="K82" t="n">
-        <v>0.7009</v>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>n_neighbors=7; weights=distance</t>
-        </is>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5244,61 +4804,6 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
-      <c r="B83" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C83" t="n">
-        <v>0.7301</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0.9867</v>
-      </c>
-      <c r="E83" t="n">
-        <v>0.7275</v>
-      </c>
-      <c r="F83" t="n">
-        <v>1</v>
-      </c>
-      <c r="G83" t="n">
-        <v>1</v>
-      </c>
-      <c r="H83" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="I83" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="J83" t="n">
-        <v>0.9796</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0.7268</v>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>n_neighbors=5; weights=distance</t>
-        </is>
-      </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5306,61 +4811,6 @@
           <t>Fold 10</t>
         </is>
       </c>
-      <c r="B84" t="n">
-        <v>0.9836</v>
-      </c>
-      <c r="C84" t="n">
-        <v>0.7341</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="E84" t="n">
-        <v>0.7208</v>
-      </c>
-      <c r="F84" t="n">
-        <v>1</v>
-      </c>
-      <c r="G84" t="n">
-        <v>1</v>
-      </c>
-      <c r="H84" t="n">
-        <v>1</v>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="n">
-        <v>0.9772999999999999</v>
-      </c>
-      <c r="K84" t="n">
-        <v>0.7276</v>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="B85" s="2" t="inlineStr">
@@ -5452,61 +4902,6 @@
           <t>Fold 1</t>
         </is>
       </c>
-      <c r="B87" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C87" t="n">
-        <v>0.9825</v>
-      </c>
-      <c r="D87" t="n">
-        <v>0.9851</v>
-      </c>
-      <c r="E87" t="n">
-        <v>0.7302</v>
-      </c>
-      <c r="F87" t="n">
-        <v>1</v>
-      </c>
-      <c r="G87" t="n">
-        <v>1</v>
-      </c>
-      <c r="H87" t="n">
-        <v>1</v>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="n">
-        <v>0.9772999999999999</v>
-      </c>
-      <c r="K87" t="n">
-        <v>0.7275</v>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
-          <t>alpha=0.01; hidden_layer_sizes=(50,)</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5514,61 +4909,6 @@
           <t>Fold 2</t>
         </is>
       </c>
-      <c r="B88" t="n">
-        <v>0.9797</v>
-      </c>
-      <c r="C88" t="n">
-        <v>0.9792</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="E88" t="n">
-        <v>0.7211</v>
-      </c>
-      <c r="F88" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="G88" t="n">
-        <v>0.9961</v>
-      </c>
-      <c r="H88" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="J88" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="K88" t="n">
-        <v>0.7296</v>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5576,61 +4916,6 @@
           <t>Fold 3</t>
         </is>
       </c>
-      <c r="B89" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="C89" t="n">
-        <v>0.9786</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0.9859</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0.731</v>
-      </c>
-      <c r="F89" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0.7499</v>
-      </c>
-      <c r="H89" t="n">
-        <v>0.9977</v>
-      </c>
-      <c r="I89" t="n">
-        <v>0.7484</v>
-      </c>
-      <c r="J89" t="n">
-        <v>0.9875</v>
-      </c>
-      <c r="K89" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5638,61 +4923,6 @@
           <t>Fold 4</t>
         </is>
       </c>
-      <c r="B90" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="C90" t="n">
-        <v>0.9842</v>
-      </c>
-      <c r="D90" t="n">
-        <v>0.9883</v>
-      </c>
-      <c r="E90" t="n">
-        <v>0.9784</v>
-      </c>
-      <c r="F90" t="n">
-        <v>1</v>
-      </c>
-      <c r="G90" t="n">
-        <v>1</v>
-      </c>
-      <c r="H90" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I90" t="n">
-        <v>0.9985000000000001</v>
-      </c>
-      <c r="J90" t="n">
-        <v>0.9851</v>
-      </c>
-      <c r="K90" t="n">
-        <v>0.7327</v>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=5</t>
-        </is>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5700,61 +4930,6 @@
           <t>Fold 5</t>
         </is>
       </c>
-      <c r="B91" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C91" t="n">
-        <v>0.7333</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0.9875</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0.7383</v>
-      </c>
-      <c r="F91" t="n">
-        <v>1</v>
-      </c>
-      <c r="G91" t="n">
-        <v>1</v>
-      </c>
-      <c r="H91" t="n">
-        <v>1</v>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="K91" t="n">
-        <v>0.7314000000000001</v>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>n_neighbors=5; weights=distance</t>
-        </is>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=10</t>
-        </is>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>max_depth=20; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5762,61 +4937,6 @@
           <t>Fold 6</t>
         </is>
       </c>
-      <c r="B92" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0.9694</v>
-      </c>
-      <c r="D92" t="n">
-        <v>0.9797</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="F92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H92" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I92" t="n">
-        <v>0.9985000000000001</v>
-      </c>
-      <c r="J92" t="n">
-        <v>0.9844000000000001</v>
-      </c>
-      <c r="K92" t="n">
-        <v>0.8918</v>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>max_depth=10; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
-        <is>
-          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5824,61 +4944,6 @@
           <t>Fold 7</t>
         </is>
       </c>
-      <c r="B93" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0.7229</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0.9836</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.7281</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0.9992</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0.7463</v>
-      </c>
-      <c r="H93" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0.7455000000000001</v>
-      </c>
-      <c r="J93" t="n">
-        <v>0.975</v>
-      </c>
-      <c r="K93" t="n">
-        <v>0.7183</v>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P93" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5886,61 +4951,6 @@
           <t>Fold 8</t>
         </is>
       </c>
-      <c r="B94" t="n">
-        <v>0.9789</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.972</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.9789</v>
-      </c>
-      <c r="E94" t="n">
-        <v>0.6986</v>
-      </c>
-      <c r="F94" t="n">
-        <v>1</v>
-      </c>
-      <c r="G94" t="n">
-        <v>1</v>
-      </c>
-      <c r="H94" t="n">
-        <v>1</v>
-      </c>
-      <c r="I94" t="n">
-        <v>1</v>
-      </c>
-      <c r="J94" t="n">
-        <v>0.9656</v>
-      </c>
-      <c r="K94" t="n">
-        <v>0.6833</v>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>n_neighbors=7; weights=distance</t>
-        </is>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=200</t>
-        </is>
-      </c>
-      <c r="P94" t="inlineStr">
-        <is>
-          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5948,121 +4958,11 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
-      <c r="B95" t="n">
-        <v>0.9828</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0.7301</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0.9867</v>
-      </c>
-      <c r="E95" t="n">
-        <v>0.7275</v>
-      </c>
-      <c r="F95" t="n">
-        <v>1</v>
-      </c>
-      <c r="G95" t="n">
-        <v>1</v>
-      </c>
-      <c r="H95" t="n">
-        <v>0.9977</v>
-      </c>
-      <c r="I95" t="n">
-        <v>0.9977</v>
-      </c>
-      <c r="J95" t="n">
-        <v>0.9843</v>
-      </c>
-      <c r="K95" t="n">
-        <v>0.7285</v>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>n_neighbors=5; weights=distance</t>
-        </is>
-      </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=5</t>
-        </is>
-      </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P95" t="inlineStr">
-        <is>
-          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
-        </is>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
           <t>Fold 10</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>0.9836</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0.7341</v>
-      </c>
-      <c r="D96" t="n">
-        <v>0.9765</v>
-      </c>
-      <c r="E96" t="n">
-        <v>0.724</v>
-      </c>
-      <c r="F96" t="n">
-        <v>1</v>
-      </c>
-      <c r="G96" t="n">
-        <v>1</v>
-      </c>
-      <c r="H96" t="n">
-        <v>0.9984</v>
-      </c>
-      <c r="I96" t="n">
-        <v>0.9985000000000001</v>
-      </c>
-      <c r="J96" t="n">
-        <v>0.9812</v>
-      </c>
-      <c r="K96" t="n">
-        <v>0.7319</v>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>C=10</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>n_neighbors=3; weights=distance</t>
-        </is>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>max_depth=None; min_samples_split=2</t>
-        </is>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>max_depth=None; n_estimators=100</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
file update onword of 8 data
</commit_message>
<xml_diff>
--- a/Results_BEFORE_filled.xlsx
+++ b/Results_BEFORE_filled.xlsx
@@ -4748,6 +4748,61 @@
           <t>Fold 1</t>
         </is>
       </c>
+      <c r="B75" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.9825</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.7294</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.9797</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.7302999999999999</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4755,6 +4810,61 @@
           <t>Fold 2</t>
         </is>
       </c>
+      <c r="B76" t="n">
+        <v>0.9797</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.9792</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.7211</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.9797</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.9734</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4762,6 +4872,61 @@
           <t>Fold 3</t>
         </is>
       </c>
+      <c r="B77" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.9786</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.9859</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.731</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.9977</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.9977</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.7318</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4769,6 +4934,61 @@
           <t>Fold 4</t>
         </is>
       </c>
+      <c r="B78" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.9842</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.9784</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.9985000000000001</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.9851</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.7327</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4776,6 +4996,61 @@
           <t>Fold 5</t>
         </is>
       </c>
+      <c r="B79" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.7333</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.9875</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.7383999999999999</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>1</v>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.7314000000000001</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4783,6 +5058,61 @@
           <t>Fold 6</t>
         </is>
       </c>
+      <c r="B80" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.9694</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.9804</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.9707</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.9985000000000001</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.9687</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4790,6 +5120,61 @@
           <t>Fold 7</t>
         </is>
       </c>
+      <c r="B81" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.7229</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.7272999999999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.7463</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.9772999999999999</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.7238</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4797,6 +5182,61 @@
           <t>Fold 8</t>
         </is>
       </c>
+      <c r="B82" t="n">
+        <v>0.9789</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.9789</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.7013</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.9703000000000001</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.7009</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>n_neighbors=7; weights=distance</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4804,6 +5244,61 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
+      <c r="B83" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.7301</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.9867</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.7275</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.9796</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.7268</v>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4811,6 +5306,61 @@
           <t>Fold 10</t>
         </is>
       </c>
+      <c r="B84" t="n">
+        <v>0.9836</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.7341</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.7208</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" t="n">
+        <v>1</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.9772999999999999</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.7276</v>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="2" t="inlineStr">
@@ -4902,6 +5452,61 @@
           <t>Fold 1</t>
         </is>
       </c>
+      <c r="B87" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.9825</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.9851</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.7302</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" t="n">
+        <v>1</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.9772999999999999</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.7275</v>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50,)</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4909,6 +5514,61 @@
           <t>Fold 2</t>
         </is>
       </c>
+      <c r="B88" t="n">
+        <v>0.9797</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.9792</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.7211</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.9961</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.7296</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4916,6 +5576,61 @@
           <t>Fold 3</t>
         </is>
       </c>
+      <c r="B89" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.9786</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.9859</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.731</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.7499</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.9977</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.7484</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.9875</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4923,6 +5638,61 @@
           <t>Fold 4</t>
         </is>
       </c>
+      <c r="B90" t="n">
+        <v>0.9836</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.9834000000000001</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.9784</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.9985000000000001</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.9851</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.7327</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=5</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4930,6 +5700,61 @@
           <t>Fold 5</t>
         </is>
       </c>
+      <c r="B91" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.7333</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.9875</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.7383</v>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+      <c r="G91" t="n">
+        <v>1</v>
+      </c>
+      <c r="H91" t="n">
+        <v>1</v>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.7314000000000001</v>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4937,6 +5762,61 @@
           <t>Fold 6</t>
         </is>
       </c>
+      <c r="B92" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.9694</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.9797</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F92" t="n">
+        <v>1</v>
+      </c>
+      <c r="G92" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0.9985000000000001</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.9844000000000001</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.8918</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>max_depth=10; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4944,6 +5824,61 @@
           <t>Fold 7</t>
         </is>
       </c>
+      <c r="B93" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.7229</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.9836</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.7281</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.9992</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.7463</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.7455000000000001</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.7183</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4951,6 +5886,61 @@
           <t>Fold 8</t>
         </is>
       </c>
+      <c r="B94" t="n">
+        <v>0.9789</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.9789</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.6986</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" t="n">
+        <v>1</v>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.9656</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.6833</v>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>n_neighbors=7; weights=distance</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4958,11 +5948,121 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
+      <c r="B95" t="n">
+        <v>0.9828</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.7301</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.9867</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.7275</v>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.9977</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.9977</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.9843</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.7285</v>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=5</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
           <t>Fold 10</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.7324000000000001</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.9765</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.9984</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.9985000000000001</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.9812</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.7319</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update code but not optimial
</commit_message>
<xml_diff>
--- a/Results_BEFORE_filled.xlsx
+++ b/Results_BEFORE_filled.xlsx
@@ -649,10 +649,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9812</v>
+        <v>0.9804</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7285</v>
+        <v>0.7276</v>
       </c>
       <c r="D5" t="n">
         <v>0.9789</v>
@@ -3341,10 +3341,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.9828</v>
+        <v>0.982</v>
       </c>
       <c r="C51" t="n">
-        <v>0.982</v>
+        <v>0.9811</v>
       </c>
       <c r="D51" t="n">
         <v>0.9867</v>
@@ -4045,10 +4045,10 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.982</v>
+        <v>0.9804</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9811</v>
+        <v>0.9792999999999999</v>
       </c>
       <c r="D63" t="n">
         <v>0.9867</v>
@@ -5307,10 +5307,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.9836</v>
+        <v>0.982</v>
       </c>
       <c r="C84" t="n">
-        <v>0.7341</v>
+        <v>0.7324000000000001</v>
       </c>
       <c r="D84" t="n">
         <v>0.9765</v>
@@ -5825,10 +5825,10 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.9765</v>
+        <v>0.9757</v>
       </c>
       <c r="C93" t="n">
-        <v>0.7229</v>
+        <v>0.722</v>
       </c>
       <c r="D93" t="n">
         <v>0.9836</v>
@@ -6156,6 +6156,61 @@
           <t>Fold 1</t>
         </is>
       </c>
+      <c r="B99" t="n">
+        <v>0.9748</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.8749</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.9721</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.9183</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.8662</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.9946</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0.9767</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.9748</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.8946</v>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>C=1</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -6163,6 +6218,61 @@
           <t>Fold 2</t>
         </is>
       </c>
+      <c r="B100" t="n">
+        <v>0.9748</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.8282</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.8625</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.9856</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.8773</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.9901</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.9023</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.9775</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.8754999999999999</v>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>C=10</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6170,6 +6280,61 @@
           <t>Fold 3</t>
         </is>
       </c>
+      <c r="B101" t="n">
+        <v>0.9766</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.8999</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.9739</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.8841</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.9838</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.8391</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.9874000000000001</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.8847</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.9336</v>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50,)</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -6177,6 +6342,61 @@
           <t>Fold 4</t>
         </is>
       </c>
+      <c r="B102" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.9649</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.8491</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.9856</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.8944</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.9320000000000001</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.8584000000000001</v>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=5</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -6184,6 +6404,61 @@
           <t>Fold 5</t>
         </is>
       </c>
+      <c r="B103" t="n">
+        <v>0.9703000000000001</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.9685</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.8649</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.9811</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.9031</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.9955000000000001</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0.9717</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0.9802</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0.9115</v>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6191,6 +6466,61 @@
           <t>Fold 6</t>
         </is>
       </c>
+      <c r="B104" t="n">
+        <v>0.9721</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.8941</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.9792999999999999</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.8935</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.8677</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.9892</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0.9022</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.9865</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0.9394</v>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6198,6 +6528,61 @@
           <t>Fold 7</t>
         </is>
       </c>
+      <c r="B105" t="n">
+        <v>0.9622000000000001</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.8342000000000001</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.9667</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.8762</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.9802</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.8566</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.9901</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0.9261</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.9792999999999999</v>
+      </c>
+      <c r="K105" t="n">
+        <v>0.8972</v>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -6205,6 +6590,61 @@
           <t>Fold 8</t>
         </is>
       </c>
+      <c r="B106" t="n">
+        <v>0.9622000000000001</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.7895</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.9694</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.9838</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.8246</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.991</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0.8822</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.9694</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0.7892</v>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>C=1</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -6212,6 +6652,61 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
+      <c r="B107" t="n">
+        <v>0.9676</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.8258</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.9631</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.8478</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.9847</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.8679</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.9937</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0.9515</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.9685</v>
+      </c>
+      <c r="K107" t="n">
+        <v>0.8401999999999999</v>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>alpha=0.01; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -6219,6 +6714,61 @@
           <t>Fold 10</t>
         </is>
       </c>
+      <c r="B108" t="n">
+        <v>0.9757</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.8705000000000001</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.9685</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.8767</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.9865</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0.9156</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.9892</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0.9316</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0.9784</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0.9147999999999999</v>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>C=1</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>n_neighbors=9; weights=distance</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="B109" s="2" t="inlineStr">
@@ -6310,6 +6860,61 @@
           <t>Fold 1</t>
         </is>
       </c>
+      <c r="B111" t="n">
+        <v>0.9397</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.5451</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.9406</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.5575</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.9478</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.532</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.9568</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0.5848</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.9451000000000001</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0.5782</v>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>n_neighbors=9; weights=distance</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50,)</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -6317,6 +6922,61 @@
           <t>Fold 2</t>
         </is>
       </c>
+      <c r="B112" t="n">
+        <v>0.9352</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.5292</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.9469</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.9451000000000001</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.4759</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.9559</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0.5591</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0.9343</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0.499</v>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50,)</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6324,6 +6984,61 @@
           <t>Fold 3</t>
         </is>
       </c>
+      <c r="B113" t="n">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.5281</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.9397</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.5224</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.9469</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.4974</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.9523</v>
+      </c>
+      <c r="I113" t="n">
+        <v>0.542</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0.946</v>
+      </c>
+      <c r="K113" t="n">
+        <v>0.5621</v>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50,)</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6331,6 +7046,61 @@
           <t>Fold 4</t>
         </is>
       </c>
+      <c r="B114" t="n">
+        <v>0.9361</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.4686</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.9433</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.4925</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.9496</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0.5336</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0.9496</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0.4824</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0.9433</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0.5067</v>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>n_neighbors=7; weights=distance</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>max_depth=10; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6338,6 +7108,61 @@
           <t>Fold 5</t>
         </is>
       </c>
+      <c r="B115" t="n">
+        <v>0.9442</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.5275</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.9442</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.5492</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.9397</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.4806</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.9568</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0.5658</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0.9496</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0.5319</v>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>n_neighbors=7; weights=distance</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6345,6 +7170,61 @@
           <t>Fold 6</t>
         </is>
       </c>
+      <c r="B116" t="n">
+        <v>0.9352</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.5248</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.9379</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.5406</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.9478</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.5667</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0.9514</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0.5499000000000001</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>C=0.01</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6352,6 +7232,61 @@
           <t>Fold 7</t>
         </is>
       </c>
+      <c r="B117" t="n">
+        <v>0.9559</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.6776</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.9505</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.5947</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.9523</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.6012999999999999</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.9595</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0.6076</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0.9577</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0.6384</v>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>n_neighbors=3; weights=distance</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6359,6 +7294,61 @@
           <t>Fold 8</t>
         </is>
       </c>
+      <c r="B118" t="n">
+        <v>0.9324</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.5308</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.9252</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.4419</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.9387</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.4699</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0.9468</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0.5046</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0.9351</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0.5127</v>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>n_neighbors=7; weights=distance</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=100</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(100,)</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6366,11 +7356,121 @@
           <t xml:space="preserve">Fold 9 </t>
         </is>
       </c>
+      <c r="B119" t="n">
+        <v>0.9351</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.5647</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.9423</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.5291</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.9514</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.5363</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0.9523</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0.5322</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0.9459</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0.5639999999999999</v>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>max_depth=20; min_samples_split=10</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>max_depth=20; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>alpha=0.0001; hidden_layer_sizes=(50, 50)</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
           <t>Fold 10</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0.9342</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.5387999999999999</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.9387</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.9405</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.4756</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0.9486</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0.5158</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0.9324</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0.4974</v>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>C=0.1</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>n_neighbors=5; weights=distance</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>max_depth=None; min_samples_split=2</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>max_depth=None; n_estimators=200</t>
+        </is>
+      </c>
+      <c r="P120" t="inlineStr">
+        <is>
+          <t>alpha=0.001; hidden_layer_sizes=(50,)</t>
         </is>
       </c>
     </row>

</xml_diff>